<commit_message>
added adjusted means to excels
</commit_message>
<xml_diff>
--- a/project-3/question_1/results/disk_intensive/disk_intensive_service_demands_utilizations.xlsx
+++ b/project-3/question_1/results/disk_intensive/disk_intensive_service_demands_utilizations.xlsx
@@ -5,19 +5,19 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Carlo\Documents\LM32\Primo anno\2o sem\TAGD\projects-repo\tagd-projects\project-3\question_1\results\disk_intensive\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Coding\TAGD\tagd-projects\project-3\question_1\results\disk_intensive\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CABDB08F-1917-4041-BC70-9DBDC4C26B82}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D7471F0-7B07-4DB5-9932-4994B2EC69F1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{426975E0-098E-4610-B47D-57C0939243CD}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{426975E0-098E-4610-B47D-57C0939243CD}"/>
   </bookViews>
   <sheets>
     <sheet name="disk_intensive_pg_stat" sheetId="2" r:id="rId1"/>
     <sheet name="Foglio1" sheetId="1" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="DatiEsterni_1" localSheetId="0" hidden="1">disk_intensive_pg_stat!$A$1:$AS$39</definedName>
+    <definedName name="DatiEsterni_1" localSheetId="0" hidden="1">disk_intensive_pg_stat!$A$1:$AT$39</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -48,7 +48,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1684" uniqueCount="282">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1686" uniqueCount="284">
   <si>
     <t>Column1</t>
   </si>
@@ -1047,12 +1047,18 @@
   <si>
     <t>Utilizzazione sistema:</t>
   </si>
+  <si>
+    <t>Column164</t>
+  </si>
+  <si>
+    <t>adjusted_mean</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1070,15 +1076,6 @@
     </font>
     <font>
       <sz val="8"/>
-      <name val="Aptos Narrow"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <u/>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -1115,11 +1112,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normale" xfId="0" builtinId="0"/>
@@ -1275,8 +1271,8 @@
 
 <file path=xl/queryTables/queryTable1.xml><?xml version="1.0" encoding="utf-8"?>
 <queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="DatiEsterni_1" connectionId="1" xr16:uid="{41469EEF-19C0-4AA4-B8E9-E41CE384874A}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0">
-  <queryTableRefresh nextId="46">
-    <queryTableFields count="45">
+  <queryTableRefresh nextId="47">
+    <queryTableFields count="46">
       <queryTableField id="1" name="Column1" tableColumnId="1"/>
       <queryTableField id="2" name="Column2" tableColumnId="2"/>
       <queryTableField id="3" name="Column3" tableColumnId="3"/>
@@ -1293,6 +1289,7 @@
       <queryTableField id="14" name="Column14" tableColumnId="14"/>
       <queryTableField id="15" name="Column15" tableColumnId="15"/>
       <queryTableField id="16" name="Column16" tableColumnId="16"/>
+      <queryTableField id="46" dataBound="0" tableColumnId="46"/>
       <queryTableField id="44" dataBound="0" tableColumnId="44"/>
       <queryTableField id="45" dataBound="0" tableColumnId="45"/>
       <queryTableField id="17" name="Column17" tableColumnId="17"/>
@@ -1328,8 +1325,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{60A95280-7C1C-4324-9CA3-848113D82398}" name="disk_intensive_pg_stat" displayName="disk_intensive_pg_stat" ref="A1:AS39" tableType="queryTable" totalsRowShown="0">
-  <autoFilter ref="A1:AS39" xr:uid="{60A95280-7C1C-4324-9CA3-848113D82398}">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{60A95280-7C1C-4324-9CA3-848113D82398}" name="disk_intensive_pg_stat" displayName="disk_intensive_pg_stat" ref="A1:AT39" tableType="queryTable" totalsRowShown="0">
+  <autoFilter ref="A1:AT39" xr:uid="{60A95280-7C1C-4324-9CA3-848113D82398}">
     <filterColumn colId="11">
       <filters>
         <filter val="82"/>
@@ -1337,7 +1334,7 @@
       </filters>
     </filterColumn>
   </autoFilter>
-  <tableColumns count="45">
+  <tableColumns count="46">
     <tableColumn id="1" xr3:uid="{06498BE1-E7DF-4186-A8BA-7EC41AD68284}" uniqueName="1" name="Column1" queryTableFieldId="1" dataDxfId="44"/>
     <tableColumn id="2" xr3:uid="{41EADF6B-D1A8-4044-97A2-F13665F34008}" uniqueName="2" name="Column2" queryTableFieldId="2" dataDxfId="43"/>
     <tableColumn id="3" xr3:uid="{7D240652-912C-4A3C-9C8A-FE54BD51214D}" uniqueName="3" name="Column3" queryTableFieldId="3" dataDxfId="42"/>
@@ -1354,6 +1351,7 @@
     <tableColumn id="14" xr3:uid="{1C876A53-EE18-42E7-96B2-863BE0F2BC4C}" uniqueName="14" name="Column14" queryTableFieldId="14" dataDxfId="31"/>
     <tableColumn id="15" xr3:uid="{0523F1B0-088A-4260-A535-1971D4AF573F}" uniqueName="15" name="Column15" queryTableFieldId="15" dataDxfId="30"/>
     <tableColumn id="16" xr3:uid="{BA909196-064F-4BCD-8FCA-D713A4392D48}" uniqueName="16" name="Column16" queryTableFieldId="16" dataDxfId="29"/>
+    <tableColumn id="46" xr3:uid="{90631FD9-D5F3-408B-BDF7-3A94B0674F27}" uniqueName="46" name="Column164" queryTableFieldId="46"/>
     <tableColumn id="44" xr3:uid="{E256130E-7AAC-47A0-881B-97790504F6A7}" uniqueName="44" name="Column162" queryTableFieldId="44" dataDxfId="28"/>
     <tableColumn id="45" xr3:uid="{B822E42B-687F-4FBB-BB28-8A85B3FC810F}" uniqueName="45" name="Column163" queryTableFieldId="45" dataDxfId="27"/>
     <tableColumn id="17" xr3:uid="{3B2C8656-2B0F-4DD6-92FE-2E37CD0111EB}" uniqueName="17" name="Column17" queryTableFieldId="17" dataDxfId="26"/>
@@ -1705,54 +1703,54 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0BB2144E-96F6-46C4-AA71-150787ACB334}">
-  <dimension ref="A1:AS46"/>
+  <dimension ref="A1:AT46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="M1" workbookViewId="0">
-      <selection activeCell="Q45" sqref="Q45"/>
+    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
+      <selection activeCell="S46" sqref="S46"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="3" width="10.6640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="20.88671875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="80.88671875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.6640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.21875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12.5546875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="12.88671875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="14.21875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="14.88671875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="11.6640625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="20.77734375" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="21.88671875" bestFit="1" customWidth="1"/>
-    <col min="15" max="16" width="20.77734375" bestFit="1" customWidth="1"/>
-    <col min="17" max="18" width="20.77734375" customWidth="1"/>
-    <col min="19" max="19" width="22.88671875" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="11.6640625" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="13.44140625" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="15.109375" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="16.5546875" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="17" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="11.6640625" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="13.44140625" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="14.88671875" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="15.33203125" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="13.6640625" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="15.5546875" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="18.77734375" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="12.44140625" bestFit="1" customWidth="1"/>
-    <col min="33" max="34" width="18.77734375" bestFit="1" customWidth="1"/>
-    <col min="35" max="38" width="11.6640625" bestFit="1" customWidth="1"/>
-    <col min="39" max="39" width="16.21875" bestFit="1" customWidth="1"/>
-    <col min="40" max="40" width="14.33203125" bestFit="1" customWidth="1"/>
-    <col min="41" max="41" width="13.33203125" bestFit="1" customWidth="1"/>
-    <col min="42" max="42" width="18.5546875" bestFit="1" customWidth="1"/>
-    <col min="43" max="43" width="17.5546875" bestFit="1" customWidth="1"/>
-    <col min="44" max="44" width="15.88671875" bestFit="1" customWidth="1"/>
-    <col min="45" max="45" width="14.88671875" bestFit="1" customWidth="1"/>
+    <col min="1" max="3" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="20.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="80.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="20.7109375" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="21.85546875" bestFit="1" customWidth="1"/>
+    <col min="15" max="16" width="20.7109375" bestFit="1" customWidth="1"/>
+    <col min="17" max="19" width="20.7109375" customWidth="1"/>
+    <col min="20" max="20" width="22.85546875" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="16.5703125" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="17" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="18.7109375" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="34" max="35" width="18.7109375" bestFit="1" customWidth="1"/>
+    <col min="36" max="39" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="40" max="40" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="41" max="41" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="42" max="42" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="43" max="43" width="18.5703125" bestFit="1" customWidth="1"/>
+    <col min="44" max="44" width="17.5703125" bestFit="1" customWidth="1"/>
+    <col min="45" max="45" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="46" max="46" width="14.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:45" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1802,94 +1800,97 @@
         <v>15</v>
       </c>
       <c r="Q1" t="s">
+        <v>282</v>
+      </c>
+      <c r="R1" t="s">
         <v>275</v>
       </c>
-      <c r="R1" t="s">
+      <c r="S1" t="s">
         <v>276</v>
       </c>
-      <c r="S1" t="s">
+      <c r="T1" t="s">
         <v>16</v>
       </c>
-      <c r="T1" t="s">
+      <c r="U1" t="s">
         <v>17</v>
       </c>
-      <c r="U1" t="s">
+      <c r="V1" t="s">
         <v>18</v>
       </c>
-      <c r="V1" t="s">
+      <c r="W1" t="s">
         <v>19</v>
       </c>
-      <c r="W1" t="s">
+      <c r="X1" t="s">
         <v>20</v>
       </c>
-      <c r="X1" t="s">
+      <c r="Y1" t="s">
         <v>21</v>
       </c>
-      <c r="Y1" t="s">
+      <c r="Z1" t="s">
         <v>22</v>
       </c>
-      <c r="Z1" t="s">
+      <c r="AA1" t="s">
         <v>23</v>
       </c>
-      <c r="AA1" t="s">
+      <c r="AB1" t="s">
         <v>24</v>
       </c>
-      <c r="AB1" t="s">
+      <c r="AC1" t="s">
         <v>25</v>
       </c>
-      <c r="AC1" t="s">
+      <c r="AD1" t="s">
         <v>26</v>
       </c>
-      <c r="AD1" t="s">
+      <c r="AE1" t="s">
         <v>27</v>
       </c>
-      <c r="AE1" t="s">
+      <c r="AF1" t="s">
         <v>28</v>
       </c>
-      <c r="AF1" t="s">
+      <c r="AG1" t="s">
         <v>29</v>
       </c>
-      <c r="AG1" t="s">
+      <c r="AH1" t="s">
         <v>30</v>
       </c>
-      <c r="AH1" t="s">
+      <c r="AI1" t="s">
         <v>31</v>
       </c>
-      <c r="AI1" t="s">
+      <c r="AJ1" t="s">
         <v>32</v>
       </c>
-      <c r="AJ1" t="s">
+      <c r="AK1" t="s">
         <v>33</v>
       </c>
-      <c r="AK1" t="s">
+      <c r="AL1" t="s">
         <v>34</v>
       </c>
-      <c r="AL1" t="s">
+      <c r="AM1" t="s">
         <v>35</v>
       </c>
-      <c r="AM1" t="s">
+      <c r="AN1" t="s">
         <v>36</v>
       </c>
-      <c r="AN1" t="s">
+      <c r="AO1" t="s">
         <v>37</v>
       </c>
-      <c r="AO1" t="s">
+      <c r="AP1" t="s">
         <v>38</v>
       </c>
-      <c r="AP1" t="s">
+      <c r="AQ1" t="s">
         <v>39</v>
       </c>
-      <c r="AQ1" t="s">
+      <c r="AR1" t="s">
         <v>40</v>
       </c>
-      <c r="AR1" t="s">
+      <c r="AS1" t="s">
         <v>41</v>
       </c>
-      <c r="AS1" t="s">
+      <c r="AT1" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="2" spans="1:45" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>43</v>
       </c>
@@ -1939,94 +1940,97 @@
         <v>58</v>
       </c>
       <c r="Q2" s="1" t="s">
+        <v>283</v>
+      </c>
+      <c r="R2" s="1" t="s">
         <v>277</v>
       </c>
-      <c r="R2" s="1" t="s">
+      <c r="S2" s="1" t="s">
         <v>278</v>
       </c>
-      <c r="S2" t="s">
+      <c r="T2" t="s">
         <v>59</v>
       </c>
-      <c r="T2" t="s">
+      <c r="U2" t="s">
         <v>60</v>
       </c>
-      <c r="U2" t="s">
+      <c r="V2" t="s">
         <v>61</v>
       </c>
-      <c r="V2" t="s">
+      <c r="W2" t="s">
         <v>62</v>
       </c>
-      <c r="W2" t="s">
+      <c r="X2" t="s">
         <v>63</v>
       </c>
-      <c r="X2" t="s">
+      <c r="Y2" t="s">
         <v>64</v>
       </c>
-      <c r="Y2" t="s">
+      <c r="Z2" t="s">
         <v>65</v>
       </c>
-      <c r="Z2" t="s">
+      <c r="AA2" t="s">
         <v>66</v>
       </c>
-      <c r="AA2" t="s">
+      <c r="AB2" t="s">
         <v>67</v>
       </c>
-      <c r="AB2" t="s">
+      <c r="AC2" t="s">
         <v>68</v>
       </c>
-      <c r="AC2" t="s">
+      <c r="AD2" t="s">
         <v>69</v>
       </c>
-      <c r="AD2" t="s">
+      <c r="AE2" t="s">
         <v>70</v>
       </c>
-      <c r="AE2" t="s">
+      <c r="AF2" t="s">
         <v>71</v>
       </c>
-      <c r="AF2" t="s">
+      <c r="AG2" t="s">
         <v>72</v>
       </c>
-      <c r="AG2" t="s">
+      <c r="AH2" t="s">
         <v>73</v>
       </c>
-      <c r="AH2" t="s">
+      <c r="AI2" t="s">
         <v>74</v>
       </c>
-      <c r="AI2" t="s">
+      <c r="AJ2" t="s">
         <v>75</v>
       </c>
-      <c r="AJ2" t="s">
+      <c r="AK2" t="s">
         <v>76</v>
       </c>
-      <c r="AK2" t="s">
+      <c r="AL2" t="s">
         <v>77</v>
       </c>
-      <c r="AL2" t="s">
+      <c r="AM2" t="s">
         <v>78</v>
       </c>
-      <c r="AM2" t="s">
+      <c r="AN2" t="s">
         <v>79</v>
       </c>
-      <c r="AN2" t="s">
+      <c r="AO2" t="s">
         <v>80</v>
       </c>
-      <c r="AO2" t="s">
+      <c r="AP2" t="s">
         <v>81</v>
       </c>
-      <c r="AP2" t="s">
+      <c r="AQ2" t="s">
         <v>82</v>
       </c>
-      <c r="AQ2" t="s">
+      <c r="AR2" t="s">
         <v>83</v>
       </c>
-      <c r="AR2" t="s">
+      <c r="AS2" t="s">
         <v>84</v>
       </c>
-      <c r="AS2" t="s">
+      <c r="AT2" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="3" spans="1:45" hidden="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:46" hidden="1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>86</v>
       </c>
@@ -2075,15 +2079,12 @@
       <c r="P3" t="s">
         <v>93</v>
       </c>
-      <c r="S3" t="s">
-        <v>91</v>
-      </c>
       <c r="T3" t="s">
+        <v>91</v>
+      </c>
+      <c r="U3" t="s">
         <v>92</v>
       </c>
-      <c r="U3" t="s">
-        <v>91</v>
-      </c>
       <c r="V3" t="s">
         <v>91</v>
       </c>
@@ -2156,8 +2157,11 @@
       <c r="AS3" t="s">
         <v>91</v>
       </c>
+      <c r="AT3" t="s">
+        <v>91</v>
+      </c>
     </row>
-    <row r="4" spans="1:45" hidden="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:46" hidden="1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>86</v>
       </c>
@@ -2206,15 +2210,12 @@
       <c r="P4" t="s">
         <v>96</v>
       </c>
-      <c r="S4" t="s">
-        <v>91</v>
-      </c>
       <c r="T4" t="s">
+        <v>91</v>
+      </c>
+      <c r="U4" t="s">
         <v>92</v>
       </c>
-      <c r="U4" t="s">
-        <v>91</v>
-      </c>
       <c r="V4" t="s">
         <v>91</v>
       </c>
@@ -2287,8 +2288,11 @@
       <c r="AS4" t="s">
         <v>91</v>
       </c>
+      <c r="AT4" t="s">
+        <v>91</v>
+      </c>
     </row>
-    <row r="5" spans="1:45" hidden="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:46" hidden="1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>86</v>
       </c>
@@ -2337,9 +2341,6 @@
       <c r="P5" t="s">
         <v>99</v>
       </c>
-      <c r="S5" t="s">
-        <v>91</v>
-      </c>
       <c r="T5" t="s">
         <v>91</v>
       </c>
@@ -2418,8 +2419,11 @@
       <c r="AS5" t="s">
         <v>91</v>
       </c>
+      <c r="AT5" t="s">
+        <v>91</v>
+      </c>
     </row>
-    <row r="6" spans="1:45" hidden="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:46" hidden="1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>86</v>
       </c>
@@ -2468,9 +2472,6 @@
       <c r="P6" t="s">
         <v>102</v>
       </c>
-      <c r="S6" t="s">
-        <v>91</v>
-      </c>
       <c r="T6" t="s">
         <v>91</v>
       </c>
@@ -2549,8 +2550,11 @@
       <c r="AS6" t="s">
         <v>91</v>
       </c>
+      <c r="AT6" t="s">
+        <v>91</v>
+      </c>
     </row>
-    <row r="7" spans="1:45" hidden="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:46" hidden="1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>86</v>
       </c>
@@ -2599,9 +2603,6 @@
       <c r="P7" t="s">
         <v>105</v>
       </c>
-      <c r="S7" t="s">
-        <v>91</v>
-      </c>
       <c r="T7" t="s">
         <v>91</v>
       </c>
@@ -2680,8 +2681,11 @@
       <c r="AS7" t="s">
         <v>91</v>
       </c>
+      <c r="AT7" t="s">
+        <v>91</v>
+      </c>
     </row>
-    <row r="8" spans="1:45" hidden="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:46" hidden="1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>86</v>
       </c>
@@ -2730,18 +2734,15 @@
       <c r="P8" t="s">
         <v>108</v>
       </c>
-      <c r="S8" t="s">
-        <v>91</v>
-      </c>
       <c r="T8" t="s">
+        <v>91</v>
+      </c>
+      <c r="U8" t="s">
         <v>109</v>
       </c>
-      <c r="U8" t="s">
+      <c r="V8" t="s">
         <v>110</v>
       </c>
-      <c r="V8" t="s">
-        <v>91</v>
-      </c>
       <c r="W8" t="s">
         <v>91</v>
       </c>
@@ -2811,8 +2812,11 @@
       <c r="AS8" t="s">
         <v>91</v>
       </c>
+      <c r="AT8" t="s">
+        <v>91</v>
+      </c>
     </row>
-    <row r="9" spans="1:45" hidden="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:46" hidden="1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>86</v>
       </c>
@@ -2861,15 +2865,12 @@
       <c r="P9" t="s">
         <v>113</v>
       </c>
-      <c r="S9" t="s">
-        <v>91</v>
-      </c>
       <c r="T9" t="s">
+        <v>91</v>
+      </c>
+      <c r="U9" t="s">
         <v>92</v>
       </c>
-      <c r="U9" t="s">
-        <v>91</v>
-      </c>
       <c r="V9" t="s">
         <v>91</v>
       </c>
@@ -2942,8 +2943,11 @@
       <c r="AS9" t="s">
         <v>91</v>
       </c>
+      <c r="AT9" t="s">
+        <v>91</v>
+      </c>
     </row>
-    <row r="10" spans="1:45" hidden="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:46" hidden="1" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>86</v>
       </c>
@@ -2992,15 +2996,12 @@
       <c r="P10" t="s">
         <v>120</v>
       </c>
-      <c r="S10" t="s">
+      <c r="T10" t="s">
         <v>121</v>
       </c>
-      <c r="T10" t="s">
+      <c r="U10" t="s">
         <v>116</v>
       </c>
-      <c r="U10" t="s">
-        <v>91</v>
-      </c>
       <c r="V10" t="s">
         <v>91</v>
       </c>
@@ -3073,8 +3074,11 @@
       <c r="AS10" t="s">
         <v>91</v>
       </c>
+      <c r="AT10" t="s">
+        <v>91</v>
+      </c>
     </row>
-    <row r="11" spans="1:45" hidden="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:46" hidden="1" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>86</v>
       </c>
@@ -3123,18 +3127,15 @@
       <c r="P11" t="s">
         <v>124</v>
       </c>
-      <c r="S11" t="s">
-        <v>91</v>
-      </c>
       <c r="T11" t="s">
+        <v>91</v>
+      </c>
+      <c r="U11" t="s">
         <v>125</v>
       </c>
-      <c r="U11" t="s">
+      <c r="V11" t="s">
         <v>126</v>
       </c>
-      <c r="V11" t="s">
-        <v>91</v>
-      </c>
       <c r="W11" t="s">
         <v>91</v>
       </c>
@@ -3204,8 +3205,11 @@
       <c r="AS11" t="s">
         <v>91</v>
       </c>
+      <c r="AT11" t="s">
+        <v>91</v>
+      </c>
     </row>
-    <row r="12" spans="1:45" hidden="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:46" hidden="1" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>86</v>
       </c>
@@ -3254,18 +3258,15 @@
       <c r="P12" t="s">
         <v>129</v>
       </c>
-      <c r="S12" t="s">
-        <v>91</v>
-      </c>
       <c r="T12" t="s">
+        <v>91</v>
+      </c>
+      <c r="U12" t="s">
         <v>130</v>
       </c>
-      <c r="U12" t="s">
+      <c r="V12" t="s">
         <v>92</v>
       </c>
-      <c r="V12" t="s">
-        <v>91</v>
-      </c>
       <c r="W12" t="s">
         <v>91</v>
       </c>
@@ -3335,8 +3336,11 @@
       <c r="AS12" t="s">
         <v>91</v>
       </c>
+      <c r="AT12" t="s">
+        <v>91</v>
+      </c>
     </row>
-    <row r="13" spans="1:45" hidden="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:46" hidden="1" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>86</v>
       </c>
@@ -3385,21 +3389,18 @@
       <c r="P13" t="s">
         <v>136</v>
       </c>
-      <c r="S13" t="s">
+      <c r="T13" t="s">
         <v>137</v>
       </c>
-      <c r="T13" t="s">
+      <c r="U13" t="s">
         <v>138</v>
       </c>
-      <c r="U13" t="s">
+      <c r="V13" t="s">
         <v>139</v>
       </c>
-      <c r="V13" t="s">
+      <c r="W13" t="s">
         <v>116</v>
       </c>
-      <c r="W13" t="s">
-        <v>91</v>
-      </c>
       <c r="X13" t="s">
         <v>91</v>
       </c>
@@ -3422,11 +3423,11 @@
         <v>91</v>
       </c>
       <c r="AE13" t="s">
+        <v>91</v>
+      </c>
+      <c r="AF13" t="s">
         <v>140</v>
       </c>
-      <c r="AF13" t="s">
-        <v>91</v>
-      </c>
       <c r="AG13" t="s">
         <v>91</v>
       </c>
@@ -3466,8 +3467,11 @@
       <c r="AS13" t="s">
         <v>91</v>
       </c>
+      <c r="AT13" t="s">
+        <v>91</v>
+      </c>
     </row>
-    <row r="14" spans="1:45" hidden="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:46" hidden="1" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>86</v>
       </c>
@@ -3516,12 +3520,9 @@
       <c r="P14" t="s">
         <v>147</v>
       </c>
-      <c r="S14" t="s">
+      <c r="T14" t="s">
         <v>148</v>
       </c>
-      <c r="T14" t="s">
-        <v>91</v>
-      </c>
       <c r="U14" t="s">
         <v>91</v>
       </c>
@@ -3597,8 +3598,11 @@
       <c r="AS14" t="s">
         <v>91</v>
       </c>
+      <c r="AT14" t="s">
+        <v>91</v>
+      </c>
     </row>
-    <row r="15" spans="1:45" hidden="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:46" hidden="1" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>86</v>
       </c>
@@ -3647,18 +3651,15 @@
       <c r="P15" t="s">
         <v>151</v>
       </c>
-      <c r="S15" t="s">
-        <v>91</v>
-      </c>
       <c r="T15" t="s">
+        <v>91</v>
+      </c>
+      <c r="U15" t="s">
         <v>125</v>
       </c>
-      <c r="U15" t="s">
+      <c r="V15" t="s">
         <v>126</v>
       </c>
-      <c r="V15" t="s">
-        <v>91</v>
-      </c>
       <c r="W15" t="s">
         <v>91</v>
       </c>
@@ -3728,8 +3729,11 @@
       <c r="AS15" t="s">
         <v>91</v>
       </c>
+      <c r="AT15" t="s">
+        <v>91</v>
+      </c>
     </row>
-    <row r="16" spans="1:45" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>86</v>
       </c>
@@ -3779,28 +3783,29 @@
         <v>158</v>
       </c>
       <c r="Q16">
-        <f>disk_intensive_pg_stat[[#This Row],[Column16]]-(disk_intensive_pg_stat[[#This Row],[Column29]]+disk_intensive_pg_stat[[#This Row],[Column30]])/disk_intensive_pg_stat[[#This Row],[Column12]]</f>
-        <v>455.1658988536588</v>
+        <f>(disk_intensive_pg_stat[[#This Row],[Column13]]-disk_intensive_pg_stat[[#This Row],[Column14]]-disk_intensive_pg_stat[[#This Row],[Column15]])/(disk_intensive_pg_stat[[#This Row],[Column12]]-2)</f>
+        <v>725.80921031249989</v>
       </c>
       <c r="R16">
+        <f>disk_intensive_pg_stat[[#This Row],[Column164]]-(disk_intensive_pg_stat[[#This Row],[Column29]]+disk_intensive_pg_stat[[#This Row],[Column30]])/disk_intensive_pg_stat[[#This Row],[Column12]]</f>
+        <v>412.16905067835472</v>
+      </c>
+      <c r="S16">
         <f>disk_intensive_pg_stat[[#This Row],[Column16]]-disk_intensive_pg_stat[[#This Row],[Column162]]</f>
-        <v>313.64015963414516</v>
-      </c>
-      <c r="S16" t="s">
+        <v>356.63700780944924</v>
+      </c>
+      <c r="T16" t="s">
         <v>159</v>
       </c>
-      <c r="T16" t="s">
+      <c r="U16" t="s">
         <v>160</v>
       </c>
-      <c r="U16" t="s">
+      <c r="V16" t="s">
         <v>161</v>
       </c>
-      <c r="V16" t="s">
+      <c r="W16" t="s">
         <v>162</v>
       </c>
-      <c r="W16" t="s">
-        <v>91</v>
-      </c>
       <c r="X16" t="s">
         <v>91</v>
       </c>
@@ -3817,26 +3822,26 @@
         <v>91</v>
       </c>
       <c r="AC16" t="s">
+        <v>91</v>
+      </c>
+      <c r="AD16" t="s">
         <v>163</v>
       </c>
-      <c r="AD16" t="s">
+      <c r="AE16" t="s">
         <v>164</v>
       </c>
-      <c r="AE16" t="s">
+      <c r="AF16" t="s">
         <v>165</v>
       </c>
-      <c r="AF16" t="s">
-        <v>91</v>
-      </c>
       <c r="AG16" t="s">
+        <v>91</v>
+      </c>
+      <c r="AH16" t="s">
         <v>166</v>
       </c>
-      <c r="AH16" t="s">
+      <c r="AI16" t="s">
         <v>167</v>
       </c>
-      <c r="AI16" t="s">
-        <v>91</v>
-      </c>
       <c r="AJ16" t="s">
         <v>91</v>
       </c>
@@ -3867,8 +3872,11 @@
       <c r="AS16" t="s">
         <v>91</v>
       </c>
+      <c r="AT16" t="s">
+        <v>91</v>
+      </c>
     </row>
-    <row r="17" spans="1:45" hidden="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:46" hidden="1" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>86</v>
       </c>
@@ -3917,21 +3925,18 @@
       <c r="P17" t="s">
         <v>173</v>
       </c>
-      <c r="S17" t="s">
+      <c r="T17" t="s">
         <v>174</v>
       </c>
-      <c r="T17" t="s">
+      <c r="U17" t="s">
         <v>175</v>
       </c>
-      <c r="U17" t="s">
+      <c r="V17" t="s">
         <v>176</v>
       </c>
-      <c r="V17" t="s">
+      <c r="W17" t="s">
         <v>116</v>
       </c>
-      <c r="W17" t="s">
-        <v>91</v>
-      </c>
       <c r="X17" t="s">
         <v>91</v>
       </c>
@@ -3954,11 +3959,11 @@
         <v>91</v>
       </c>
       <c r="AE17" t="s">
+        <v>91</v>
+      </c>
+      <c r="AF17" t="s">
         <v>177</v>
       </c>
-      <c r="AF17" t="s">
-        <v>91</v>
-      </c>
       <c r="AG17" t="s">
         <v>91</v>
       </c>
@@ -3998,8 +4003,11 @@
       <c r="AS17" t="s">
         <v>91</v>
       </c>
+      <c r="AT17" t="s">
+        <v>91</v>
+      </c>
     </row>
-    <row r="18" spans="1:45" hidden="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:46" hidden="1" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>86</v>
       </c>
@@ -4048,9 +4056,6 @@
       <c r="P18" t="s">
         <v>180</v>
       </c>
-      <c r="S18" t="s">
-        <v>91</v>
-      </c>
       <c r="T18" t="s">
         <v>91</v>
       </c>
@@ -4129,8 +4134,11 @@
       <c r="AS18" t="s">
         <v>91</v>
       </c>
+      <c r="AT18" t="s">
+        <v>91</v>
+      </c>
     </row>
-    <row r="19" spans="1:45" hidden="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:46" hidden="1" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>86</v>
       </c>
@@ -4179,21 +4187,18 @@
       <c r="P19" t="s">
         <v>183</v>
       </c>
-      <c r="S19" t="s">
-        <v>91</v>
-      </c>
       <c r="T19" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="U19" t="s">
         <v>92</v>
       </c>
       <c r="V19" t="s">
+        <v>92</v>
+      </c>
+      <c r="W19" t="s">
         <v>116</v>
       </c>
-      <c r="W19" t="s">
-        <v>91</v>
-      </c>
       <c r="X19" t="s">
         <v>91</v>
       </c>
@@ -4216,11 +4221,11 @@
         <v>91</v>
       </c>
       <c r="AE19" t="s">
+        <v>91</v>
+      </c>
+      <c r="AF19" t="s">
         <v>184</v>
       </c>
-      <c r="AF19" t="s">
-        <v>91</v>
-      </c>
       <c r="AG19" t="s">
         <v>91</v>
       </c>
@@ -4260,8 +4265,11 @@
       <c r="AS19" t="s">
         <v>91</v>
       </c>
+      <c r="AT19" t="s">
+        <v>91</v>
+      </c>
     </row>
-    <row r="20" spans="1:45" hidden="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:46" hidden="1" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>86</v>
       </c>
@@ -4310,21 +4318,18 @@
       <c r="P20" t="s">
         <v>187</v>
       </c>
-      <c r="S20" t="s">
-        <v>91</v>
-      </c>
       <c r="T20" t="s">
+        <v>91</v>
+      </c>
+      <c r="U20" t="s">
         <v>109</v>
       </c>
-      <c r="U20" t="s">
+      <c r="V20" t="s">
         <v>188</v>
       </c>
-      <c r="V20" t="s">
+      <c r="W20" t="s">
         <v>189</v>
       </c>
-      <c r="W20" t="s">
-        <v>91</v>
-      </c>
       <c r="X20" t="s">
         <v>91</v>
       </c>
@@ -4347,11 +4352,11 @@
         <v>91</v>
       </c>
       <c r="AE20" t="s">
+        <v>91</v>
+      </c>
+      <c r="AF20" t="s">
         <v>190</v>
       </c>
-      <c r="AF20" t="s">
-        <v>91</v>
-      </c>
       <c r="AG20" t="s">
         <v>91</v>
       </c>
@@ -4391,8 +4396,11 @@
       <c r="AS20" t="s">
         <v>91</v>
       </c>
+      <c r="AT20" t="s">
+        <v>91</v>
+      </c>
     </row>
-    <row r="21" spans="1:45" hidden="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:46" hidden="1" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>86</v>
       </c>
@@ -4441,15 +4449,12 @@
       <c r="P21" t="s">
         <v>193</v>
       </c>
-      <c r="S21" t="s">
-        <v>91</v>
-      </c>
       <c r="T21" t="s">
+        <v>91</v>
+      </c>
+      <c r="U21" t="s">
         <v>92</v>
       </c>
-      <c r="U21" t="s">
-        <v>91</v>
-      </c>
       <c r="V21" t="s">
         <v>91</v>
       </c>
@@ -4522,8 +4527,11 @@
       <c r="AS21" t="s">
         <v>91</v>
       </c>
+      <c r="AT21" t="s">
+        <v>91</v>
+      </c>
     </row>
-    <row r="22" spans="1:45" hidden="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:46" hidden="1" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>86</v>
       </c>
@@ -4572,15 +4580,12 @@
       <c r="P22" t="s">
         <v>196</v>
       </c>
-      <c r="S22" t="s">
-        <v>91</v>
-      </c>
       <c r="T22" t="s">
+        <v>91</v>
+      </c>
+      <c r="U22" t="s">
         <v>92</v>
       </c>
-      <c r="U22" t="s">
-        <v>91</v>
-      </c>
       <c r="V22" t="s">
         <v>91</v>
       </c>
@@ -4653,8 +4658,11 @@
       <c r="AS22" t="s">
         <v>91</v>
       </c>
+      <c r="AT22" t="s">
+        <v>91</v>
+      </c>
     </row>
-    <row r="23" spans="1:45" hidden="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:46" hidden="1" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>86</v>
       </c>
@@ -4703,18 +4711,15 @@
       <c r="P23" t="s">
         <v>199</v>
       </c>
-      <c r="S23" t="s">
-        <v>91</v>
-      </c>
       <c r="T23" t="s">
+        <v>91</v>
+      </c>
+      <c r="U23" t="s">
         <v>109</v>
       </c>
-      <c r="U23" t="s">
+      <c r="V23" t="s">
         <v>200</v>
       </c>
-      <c r="V23" t="s">
-        <v>91</v>
-      </c>
       <c r="W23" t="s">
         <v>91</v>
       </c>
@@ -4784,8 +4789,11 @@
       <c r="AS23" t="s">
         <v>91</v>
       </c>
+      <c r="AT23" t="s">
+        <v>91</v>
+      </c>
     </row>
-    <row r="24" spans="1:45" hidden="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:46" hidden="1" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>86</v>
       </c>
@@ -4834,18 +4842,15 @@
       <c r="P24" t="s">
         <v>203</v>
       </c>
-      <c r="S24" t="s">
-        <v>91</v>
-      </c>
       <c r="T24" t="s">
+        <v>91</v>
+      </c>
+      <c r="U24" t="s">
         <v>204</v>
       </c>
-      <c r="U24" t="s">
+      <c r="V24" t="s">
         <v>92</v>
       </c>
-      <c r="V24" t="s">
-        <v>91</v>
-      </c>
       <c r="W24" t="s">
         <v>91</v>
       </c>
@@ -4915,8 +4920,11 @@
       <c r="AS24" t="s">
         <v>91</v>
       </c>
+      <c r="AT24" t="s">
+        <v>91</v>
+      </c>
     </row>
-    <row r="25" spans="1:45" hidden="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:46" hidden="1" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>86</v>
       </c>
@@ -4965,18 +4973,15 @@
       <c r="P25" t="s">
         <v>207</v>
       </c>
-      <c r="S25" t="s">
-        <v>91</v>
-      </c>
       <c r="T25" t="s">
+        <v>91</v>
+      </c>
+      <c r="U25" t="s">
         <v>92</v>
       </c>
-      <c r="U25" t="s">
+      <c r="V25" t="s">
         <v>204</v>
       </c>
-      <c r="V25" t="s">
-        <v>91</v>
-      </c>
       <c r="W25" t="s">
         <v>91</v>
       </c>
@@ -5046,8 +5051,11 @@
       <c r="AS25" t="s">
         <v>91</v>
       </c>
+      <c r="AT25" t="s">
+        <v>91</v>
+      </c>
     </row>
-    <row r="26" spans="1:45" hidden="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:46" hidden="1" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>86</v>
       </c>
@@ -5096,9 +5104,6 @@
       <c r="P26" t="s">
         <v>210</v>
       </c>
-      <c r="S26" t="s">
-        <v>91</v>
-      </c>
       <c r="T26" t="s">
         <v>91</v>
       </c>
@@ -5177,8 +5182,11 @@
       <c r="AS26" t="s">
         <v>91</v>
       </c>
+      <c r="AT26" t="s">
+        <v>91</v>
+      </c>
     </row>
-    <row r="27" spans="1:45" hidden="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:46" hidden="1" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>86</v>
       </c>
@@ -5227,18 +5235,15 @@
       <c r="P27" t="s">
         <v>213</v>
       </c>
-      <c r="S27" t="s">
-        <v>91</v>
-      </c>
       <c r="T27" t="s">
+        <v>91</v>
+      </c>
+      <c r="U27" t="s">
         <v>116</v>
       </c>
-      <c r="U27" t="s">
+      <c r="V27" t="s">
         <v>214</v>
       </c>
-      <c r="V27" t="s">
-        <v>91</v>
-      </c>
       <c r="W27" t="s">
         <v>91</v>
       </c>
@@ -5308,8 +5313,11 @@
       <c r="AS27" t="s">
         <v>91</v>
       </c>
+      <c r="AT27" t="s">
+        <v>91</v>
+      </c>
     </row>
-    <row r="28" spans="1:45" hidden="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:46" hidden="1" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>86</v>
       </c>
@@ -5358,9 +5366,6 @@
       <c r="P28" t="s">
         <v>217</v>
       </c>
-      <c r="S28" t="s">
-        <v>91</v>
-      </c>
       <c r="T28" t="s">
         <v>91</v>
       </c>
@@ -5439,8 +5444,11 @@
       <c r="AS28" t="s">
         <v>91</v>
       </c>
+      <c r="AT28" t="s">
+        <v>91</v>
+      </c>
     </row>
-    <row r="29" spans="1:45" hidden="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:46" hidden="1" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>86</v>
       </c>
@@ -5489,17 +5497,14 @@
       <c r="P29" t="s">
         <v>220</v>
       </c>
-      <c r="S29" t="s">
-        <v>91</v>
-      </c>
       <c r="T29" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="U29" t="s">
         <v>92</v>
       </c>
       <c r="V29" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="W29" t="s">
         <v>91</v>
@@ -5570,8 +5575,11 @@
       <c r="AS29" t="s">
         <v>91</v>
       </c>
+      <c r="AT29" t="s">
+        <v>91</v>
+      </c>
     </row>
-    <row r="30" spans="1:45" hidden="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:46" hidden="1" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>86</v>
       </c>
@@ -5620,21 +5628,18 @@
       <c r="P30" t="s">
         <v>223</v>
       </c>
-      <c r="S30" t="s">
-        <v>91</v>
-      </c>
       <c r="T30" t="s">
-        <v>224</v>
+        <v>91</v>
       </c>
       <c r="U30" t="s">
         <v>224</v>
       </c>
       <c r="V30" t="s">
+        <v>224</v>
+      </c>
+      <c r="W30" t="s">
         <v>92</v>
       </c>
-      <c r="W30" t="s">
-        <v>91</v>
-      </c>
       <c r="X30" t="s">
         <v>91</v>
       </c>
@@ -5657,11 +5662,11 @@
         <v>91</v>
       </c>
       <c r="AE30" t="s">
+        <v>91</v>
+      </c>
+      <c r="AF30" t="s">
         <v>225</v>
       </c>
-      <c r="AF30" t="s">
-        <v>91</v>
-      </c>
       <c r="AG30" t="s">
         <v>91</v>
       </c>
@@ -5701,8 +5706,11 @@
       <c r="AS30" t="s">
         <v>91</v>
       </c>
+      <c r="AT30" t="s">
+        <v>91</v>
+      </c>
     </row>
-    <row r="31" spans="1:45" hidden="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:46" hidden="1" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>86</v>
       </c>
@@ -5751,21 +5759,18 @@
       <c r="P31" t="s">
         <v>228</v>
       </c>
-      <c r="S31" t="s">
-        <v>91</v>
-      </c>
       <c r="T31" t="s">
+        <v>91</v>
+      </c>
+      <c r="U31" t="s">
         <v>92</v>
       </c>
-      <c r="U31" t="s">
+      <c r="V31" t="s">
         <v>143</v>
       </c>
-      <c r="V31" t="s">
+      <c r="W31" t="s">
         <v>92</v>
       </c>
-      <c r="W31" t="s">
-        <v>91</v>
-      </c>
       <c r="X31" t="s">
         <v>91</v>
       </c>
@@ -5788,11 +5793,11 @@
         <v>91</v>
       </c>
       <c r="AE31" t="s">
+        <v>91</v>
+      </c>
+      <c r="AF31" t="s">
         <v>229</v>
       </c>
-      <c r="AF31" t="s">
-        <v>91</v>
-      </c>
       <c r="AG31" t="s">
         <v>91</v>
       </c>
@@ -5832,8 +5837,11 @@
       <c r="AS31" t="s">
         <v>91</v>
       </c>
+      <c r="AT31" t="s">
+        <v>91</v>
+      </c>
     </row>
-    <row r="32" spans="1:45" hidden="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:46" hidden="1" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>86</v>
       </c>
@@ -5882,21 +5890,18 @@
       <c r="P32" t="s">
         <v>235</v>
       </c>
-      <c r="S32" t="s">
+      <c r="T32" t="s">
         <v>236</v>
       </c>
-      <c r="T32" t="s">
+      <c r="U32" t="s">
         <v>200</v>
       </c>
-      <c r="U32" t="s">
+      <c r="V32" t="s">
         <v>237</v>
       </c>
-      <c r="V32" t="s">
+      <c r="W32" t="s">
         <v>204</v>
       </c>
-      <c r="W32" t="s">
-        <v>91</v>
-      </c>
       <c r="X32" t="s">
         <v>91</v>
       </c>
@@ -5919,11 +5924,11 @@
         <v>91</v>
       </c>
       <c r="AE32" t="s">
+        <v>91</v>
+      </c>
+      <c r="AF32" t="s">
         <v>238</v>
       </c>
-      <c r="AF32" t="s">
-        <v>91</v>
-      </c>
       <c r="AG32" t="s">
         <v>91</v>
       </c>
@@ -5963,8 +5968,11 @@
       <c r="AS32" t="s">
         <v>91</v>
       </c>
+      <c r="AT32" t="s">
+        <v>91</v>
+      </c>
     </row>
-    <row r="33" spans="1:45" hidden="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:46" hidden="1" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>86</v>
       </c>
@@ -6013,15 +6021,12 @@
       <c r="P33" t="s">
         <v>241</v>
       </c>
-      <c r="S33" t="s">
-        <v>91</v>
-      </c>
       <c r="T33" t="s">
+        <v>91</v>
+      </c>
+      <c r="U33" t="s">
         <v>92</v>
       </c>
-      <c r="U33" t="s">
-        <v>91</v>
-      </c>
       <c r="V33" t="s">
         <v>91</v>
       </c>
@@ -6094,8 +6099,11 @@
       <c r="AS33" t="s">
         <v>91</v>
       </c>
+      <c r="AT33" t="s">
+        <v>91</v>
+      </c>
     </row>
-    <row r="34" spans="1:45" hidden="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:46" hidden="1" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>86</v>
       </c>
@@ -6144,12 +6152,9 @@
       <c r="P34" t="s">
         <v>247</v>
       </c>
-      <c r="S34" t="s">
+      <c r="T34" t="s">
         <v>248</v>
       </c>
-      <c r="T34" t="s">
-        <v>91</v>
-      </c>
       <c r="U34" t="s">
         <v>91</v>
       </c>
@@ -6225,8 +6230,11 @@
       <c r="AS34" t="s">
         <v>91</v>
       </c>
+      <c r="AT34" t="s">
+        <v>91</v>
+      </c>
     </row>
-    <row r="35" spans="1:45" hidden="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:46" hidden="1" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>86</v>
       </c>
@@ -6275,18 +6283,15 @@
       <c r="P35" t="s">
         <v>254</v>
       </c>
-      <c r="S35" t="s">
+      <c r="T35" t="s">
         <v>255</v>
       </c>
-      <c r="T35" t="s">
+      <c r="U35" t="s">
         <v>109</v>
       </c>
-      <c r="U35" t="s">
+      <c r="V35" t="s">
         <v>256</v>
       </c>
-      <c r="V35" t="s">
-        <v>91</v>
-      </c>
       <c r="W35" t="s">
         <v>91</v>
       </c>
@@ -6356,8 +6361,11 @@
       <c r="AS35" t="s">
         <v>91</v>
       </c>
+      <c r="AT35" t="s">
+        <v>91</v>
+      </c>
     </row>
-    <row r="36" spans="1:45" hidden="1" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:46" hidden="1" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>86</v>
       </c>
@@ -6406,17 +6414,14 @@
       <c r="P36" t="s">
         <v>259</v>
       </c>
-      <c r="S36" t="s">
-        <v>91</v>
-      </c>
       <c r="T36" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="U36" t="s">
         <v>92</v>
       </c>
       <c r="V36" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="W36" t="s">
         <v>91</v>
@@ -6487,8 +6492,11 @@
       <c r="AS36" t="s">
         <v>91</v>
       </c>
+      <c r="AT36" t="s">
+        <v>91</v>
+      </c>
     </row>
-    <row r="37" spans="1:45" hidden="1" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:46" hidden="1" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>86</v>
       </c>
@@ -6537,12 +6545,9 @@
       <c r="P37" t="s">
         <v>265</v>
       </c>
-      <c r="S37" t="s">
+      <c r="T37" t="s">
         <v>266</v>
       </c>
-      <c r="T37" t="s">
-        <v>91</v>
-      </c>
       <c r="U37" t="s">
         <v>91</v>
       </c>
@@ -6618,8 +6623,11 @@
       <c r="AS37" t="s">
         <v>91</v>
       </c>
+      <c r="AT37" t="s">
+        <v>91</v>
+      </c>
     </row>
-    <row r="38" spans="1:45" hidden="1" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:46" hidden="1" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>86</v>
       </c>
@@ -6668,21 +6676,18 @@
       <c r="P38" t="s">
         <v>269</v>
       </c>
-      <c r="S38" t="s">
-        <v>91</v>
-      </c>
       <c r="T38" t="s">
+        <v>91</v>
+      </c>
+      <c r="U38" t="s">
         <v>92</v>
       </c>
-      <c r="U38" t="s">
+      <c r="V38" t="s">
         <v>86</v>
       </c>
-      <c r="V38" t="s">
+      <c r="W38" t="s">
         <v>143</v>
       </c>
-      <c r="W38" t="s">
-        <v>91</v>
-      </c>
       <c r="X38" t="s">
         <v>91</v>
       </c>
@@ -6705,11 +6710,11 @@
         <v>91</v>
       </c>
       <c r="AE38" t="s">
+        <v>91</v>
+      </c>
+      <c r="AF38" t="s">
         <v>270</v>
       </c>
-      <c r="AF38" t="s">
-        <v>91</v>
-      </c>
       <c r="AG38" t="s">
         <v>91</v>
       </c>
@@ -6749,8 +6754,11 @@
       <c r="AS38" t="s">
         <v>91</v>
       </c>
+      <c r="AT38" t="s">
+        <v>91</v>
+      </c>
     </row>
-    <row r="39" spans="1:45" hidden="1" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:46" hidden="1" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>86</v>
       </c>
@@ -6799,21 +6807,18 @@
       <c r="P39" t="s">
         <v>273</v>
       </c>
-      <c r="S39" t="s">
-        <v>91</v>
-      </c>
       <c r="T39" t="s">
+        <v>91</v>
+      </c>
+      <c r="U39" t="s">
         <v>92</v>
       </c>
-      <c r="U39" t="s">
+      <c r="V39" t="s">
         <v>116</v>
       </c>
-      <c r="V39" t="s">
+      <c r="W39" t="s">
         <v>92</v>
       </c>
-      <c r="W39" t="s">
-        <v>91</v>
-      </c>
       <c r="X39" t="s">
         <v>91</v>
       </c>
@@ -6836,11 +6841,11 @@
         <v>91</v>
       </c>
       <c r="AE39" t="s">
+        <v>91</v>
+      </c>
+      <c r="AF39" t="s">
         <v>274</v>
       </c>
-      <c r="AF39" t="s">
-        <v>91</v>
-      </c>
       <c r="AG39" t="s">
         <v>91</v>
       </c>
@@ -6880,34 +6885,37 @@
       <c r="AS39" t="s">
         <v>91</v>
       </c>
+      <c r="AT39" t="s">
+        <v>91</v>
+      </c>
     </row>
-    <row r="42" spans="1:45" x14ac:dyDescent="0.3">
-      <c r="Q42" s="1" t="s">
+    <row r="42" spans="1:46" x14ac:dyDescent="0.25">
+      <c r="R42" s="1" t="s">
         <v>279</v>
       </c>
-      <c r="R42" s="1" t="s">
+      <c r="S42" s="1" t="s">
         <v>280</v>
       </c>
     </row>
-    <row r="43" spans="1:45" x14ac:dyDescent="0.3">
-      <c r="Q43" s="2">
-        <f>0.4551658989*1.31147835036402</f>
-        <v>0.59694022223132825</v>
-      </c>
-      <c r="R43">
-        <f>0.3136401596*1.31147835036402</f>
-        <v>0.41133227912011594</v>
+    <row r="43" spans="1:46" x14ac:dyDescent="0.25">
+      <c r="R43" s="2">
+        <f>R16/1000*1.31147835036402</f>
+        <v>0.54055078665475276</v>
+      </c>
+      <c r="S43">
+        <f>S16/1000*1.31147835036402</f>
+        <v>0.46772171468069657</v>
       </c>
     </row>
-    <row r="45" spans="1:45" x14ac:dyDescent="0.3">
-      <c r="Q45" s="3" t="s">
+    <row r="45" spans="1:46" x14ac:dyDescent="0.25">
+      <c r="R45" s="1" t="s">
         <v>281</v>
       </c>
     </row>
-    <row r="46" spans="1:45" x14ac:dyDescent="0.3">
-      <c r="Q46">
-        <f>Q43+R43</f>
-        <v>1.0082725013514442</v>
+    <row r="46" spans="1:46" x14ac:dyDescent="0.25">
+      <c r="R46">
+        <f>R43+S43</f>
+        <v>1.0082725013354494</v>
       </c>
     </row>
   </sheetData>
@@ -6925,7 +6933,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>